<commit_message>
Updated Story to Chapter 118
</commit_message>
<xml_diff>
--- a/DeathTrap Dungeon Map.xlsx
+++ b/DeathTrap Dungeon Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k_zeb\Documents\2018-2019 School Year\Semester 2\ICS3U\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2018-2019 School Year\Semester 2\ICS3U\CPT\CPT2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F72D985-0C45-401D-B64A-DC8CF12B6174}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC4C04C-50DA-4F84-B8BD-288375463432}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{85B14AB0-DF22-4A1D-AF82-67BF0BF00D36}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="2400" windowHeight="585" xr2:uid="{85B14AB0-DF22-4A1D-AF82-67BF0BF00D36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="155">
   <si>
     <t>Exit</t>
   </si>
@@ -289,6 +289,213 @@
   </si>
   <si>
     <t>146, 219</t>
+  </si>
+  <si>
+    <t>271, 30, 212</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Manticore poem</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>Skill -2</t>
+  </si>
+  <si>
+    <t>126, 83</t>
+  </si>
+  <si>
+    <t>Option one only if not searched Barbarian</t>
+  </si>
+  <si>
+    <t>265, 300, 327</t>
+  </si>
+  <si>
+    <t>Option one only if have Ring of Wishes</t>
+  </si>
+  <si>
+    <t>52, 369</t>
+  </si>
+  <si>
+    <t>rubbed liquid in wounds</t>
+  </si>
+  <si>
+    <t>Option one only if not opened red book</t>
+  </si>
+  <si>
+    <t>317, 117</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>Scorpion, Manticore, No</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>301, 142</t>
+  </si>
+  <si>
+    <t>106, 383</t>
+  </si>
+  <si>
+    <t>313</t>
+  </si>
+  <si>
+    <t>307, 263, 136</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>152, 121</t>
+  </si>
+  <si>
+    <t>Roll two dice, compare against 8</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>381</t>
+  </si>
+  <si>
+    <t>343, 268</t>
+  </si>
+  <si>
+    <t>54, 261</t>
+  </si>
+  <si>
+    <t>Bloodbeast description</t>
+  </si>
+  <si>
+    <t>172, 357</t>
+  </si>
+  <si>
+    <t>Read Bloodbeast description</t>
+  </si>
+  <si>
+    <t>257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Orc, 5, 5, Second Orc, 6, 4 </t>
+  </si>
+  <si>
+    <t>Skill -4 only for this fight.</t>
+  </si>
+  <si>
+    <t>284, 230</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>opal-studded dagger</t>
+  </si>
+  <si>
+    <t>248</t>
+  </si>
+  <si>
+    <t>iron shield</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>105, 235</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>266, 305</t>
+  </si>
+  <si>
+    <t>87, 217</t>
+  </si>
+  <si>
+    <t>133, 251</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>Goblet</t>
+  </si>
+  <si>
+    <t>Option one if not searched Barbarian</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>Doppelganger Potion</t>
+  </si>
+  <si>
+    <t>168, 267</t>
+  </si>
+  <si>
+    <t>394,59,14</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>43, 24</t>
+  </si>
+  <si>
+    <t>58,223</t>
+  </si>
+  <si>
+    <t>267</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>Provisions-2</t>
+  </si>
+  <si>
+    <t>371, 74</t>
+  </si>
+  <si>
+    <t>Ball thrown</t>
+  </si>
+  <si>
+    <t>Option one only if ball thrown &lt;2</t>
+  </si>
+  <si>
+    <t>336, 298</t>
+  </si>
+  <si>
+    <t>Ring on</t>
+  </si>
+  <si>
+    <t>Stamina +3</t>
+  </si>
+  <si>
+    <t>329, 135</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -644,59 +851,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB858960-B3EB-46C4-ADC9-7102045BD3E6}">
-  <dimension ref="A1:H401"/>
+  <dimension ref="A1:I401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
+      <selection pane="bottomRight" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -704,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -712,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -720,29 +934,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>364</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -750,7 +964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -758,29 +972,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -788,34 +1005,46 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -823,18 +1052,21 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -842,18 +1074,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -861,41 +1093,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -903,15 +1138,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -919,18 +1157,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -938,18 +1176,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -957,29 +1195,29 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -987,21 +1225,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1009,100 +1247,112 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1110,18 +1360,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1129,18 +1379,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1148,15 +1398,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1164,37 +1417,46 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1202,64 +1464,76 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="C56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I56" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -1267,15 +1541,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -1283,343 +1560,631 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="I65" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
Update DeathTrap Dungeon Map.xlsx
</commit_message>
<xml_diff>
--- a/DeathTrap Dungeon Map.xlsx
+++ b/DeathTrap Dungeon Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2018-2019 School Year\Semester 2\ICS3U\CPT\CPT2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD77E919-FB9C-47FA-BA44-5A37D50B5BF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0282CB2-0CD2-408E-8DA9-1CC3DCAF5F8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27570" yWindow="5970" windowWidth="2400" windowHeight="585" xr2:uid="{85B14AB0-DF22-4A1D-AF82-67BF0BF00D36}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="240">
   <si>
     <t>Exit</t>
   </si>
@@ -666,9 +666,6 @@
     <t>1st Flying Guardian, 7, 8, 2nd Flying Guardian, 8, 8</t>
   </si>
   <si>
-    <t>One at a time</t>
-  </si>
-  <si>
     <t>Roll 2 dice, compare to Skill</t>
   </si>
   <si>
@@ -697,6 +694,63 @@
   </si>
   <si>
     <t>275</t>
+  </si>
+  <si>
+    <t>294, 334</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Lose all gems</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>iron key, sapphire</t>
+  </si>
+  <si>
+    <t>361, 302</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>299, 83</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>stilts</t>
+  </si>
+  <si>
+    <t>use coin</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>One at a time, skill -2 for fight</t>
+  </si>
+  <si>
+    <t>Skill -3 for fight, one at a time</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>Stamina-4</t>
+  </si>
+  <si>
+    <t>94, 267</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1109,10 @@
   <dimension ref="A1:I401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B160" sqref="B160"/>
+      <selection pane="bottomRight" activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,7 +2788,7 @@
         <v>210</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -2745,7 +2799,7 @@
         <v>21</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2753,13 +2807,13 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -2767,7 +2821,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -2775,7 +2829,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>101</v>
@@ -2786,7 +2840,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>101</v>
@@ -2797,13 +2851,13 @@
         <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D158" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D158" s="2" t="s">
+      <c r="I158" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="I158" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -2811,7 +2865,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>59</v>
@@ -2821,83 +2875,149 @@
       <c r="A160" s="1">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I162" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I163" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D166" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>

</xml_diff>